<commit_message>
EffNetV2M_class 11개 추가_test acc 91.68%
</commit_message>
<xml_diff>
--- a/model_summary_10epoch.xlsx
+++ b/model_summary_10epoch.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PythonWorkspace\220307-0715_AI전문가과정\AI_project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Documents\작업방\AI교육\팀프로젝트\GitHub\AI_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0E19D84-7F11-49A3-8302-F368DBFC9E62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="372" yWindow="0" windowWidth="11412" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="370" yWindow="0" windowWidth="11410" windowHeight="8880"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>개발일시</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -72,16 +71,19 @@
   </si>
   <si>
     <t>Class개수</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>박영서</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="177" formatCode="yymmdd;@"/>
-    <numFmt numFmtId="182" formatCode="0.0000_ "/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="177" formatCode="0.0000_ "/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -160,11 +162,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -447,26 +449,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.65"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="7.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.84765625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.8984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.8984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.09765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.44921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.9140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.9140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.08203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.4140625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.84765625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.796875" style="4"/>
+    <col min="8" max="8" width="7.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.65">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -491,9 +495,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.65">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" s="5">
-        <v>44720</v>
+        <v>220608</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
@@ -515,6 +519,32 @@
       </c>
       <c r="H2" s="3">
         <v>7.6215036213397896E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A3" s="5">
+        <v>220609</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="2">
+        <v>11</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.91920000000000002</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.91679999999999995</v>
+      </c>
+      <c r="G3" s="3">
+        <v>0.46300000000000002</v>
+      </c>
+      <c r="H3" s="3">
+        <v>0.37890000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
VGG16_class 11개 추가_test acc 84.15%
</commit_message>
<xml_diff>
--- a/model_summary_10epoch.xlsx
+++ b/model_summary_10epoch.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>개발일시</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -75,6 +75,10 @@
   </si>
   <si>
     <t>박영서</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>VGG16</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -83,7 +87,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="177" formatCode="0.0000_ "/>
+    <numFmt numFmtId="176" formatCode="0.0000_ "/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -162,7 +166,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -450,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.45"/>
@@ -547,6 +551,32 @@
         <v>0.37890000000000001</v>
       </c>
     </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A4" s="5">
+        <v>220609</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="2">
+        <v>11</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.84940000000000004</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.84150000000000003</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0.65500000000000003</v>
+      </c>
+      <c r="H4" s="3">
+        <v>0.71160000000000001</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
MobileNetV2_class 11개 추가_test acc 85.75%
</commit_message>
<xml_diff>
--- a/model_summary_10epoch.xlsx
+++ b/model_summary_10epoch.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>개발일시</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -79,6 +79,10 @@
   </si>
   <si>
     <t>VGG16</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MobileNetV2</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -454,17 +458,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="G5" sqref="G5:H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="7.5" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.9140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" style="2" customWidth="1"/>
     <col min="4" max="4" width="7.9140625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.08203125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.4140625" style="1" bestFit="1" customWidth="1"/>
@@ -577,6 +581,32 @@
         <v>0.71160000000000001</v>
       </c>
     </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A5" s="5">
+        <v>220609</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="2">
+        <v>11</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.86639999999999995</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.85750000000000004</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0.51559999999999995</v>
+      </c>
+      <c r="H5" s="3">
+        <v>0.51290000000000002</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>